<commit_message>
[Ankur Yadav] expense management Task
</commit_message>
<xml_diff>
--- a/data/excel/CamSbtExpenseManagement.xlsx
+++ b/data/excel/CamSbtExpenseManagement.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\projectQuadlabs\data\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ankur.Yadav\git\ProjectQuadlabs\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC2B4DD-52CA-40D8-9143-6C0773DCEC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F879B3-DD7A-4C8B-AFF8-8EEF863CB1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PerDiemAllowance" sheetId="2" r:id="rId1"/>
-    <sheet name="ConveyanceAllowance" sheetId="3" r:id="rId2"/>
-    <sheet name="CategoriesAndPolicies" sheetId="4" r:id="rId3"/>
-    <sheet name="BudgetManagemnet" sheetId="5" r:id="rId4"/>
+    <sheet name="PerDiemAllowance1" sheetId="7" r:id="rId2"/>
+    <sheet name="ConveyanceAllowance" sheetId="3" r:id="rId3"/>
+    <sheet name="CategoriesAndPolicies" sheetId="4" r:id="rId4"/>
+    <sheet name="BudgetManagemnet" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="76">
   <si>
     <t>Source</t>
   </si>
@@ -48,9 +50,6 @@
     <t>sbt</t>
   </si>
   <si>
-    <t>//staging117/sbt</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
@@ -120,15 +119,9 @@
     <t>ConveyanceAllowanceName</t>
   </si>
   <si>
-    <t>Bus</t>
-  </si>
-  <si>
     <t>RatePer</t>
   </si>
   <si>
-    <t>KM</t>
-  </si>
-  <si>
     <t>RateAmount</t>
   </si>
   <si>
@@ -195,10 +188,76 @@
     <t>Account,Team</t>
   </si>
   <si>
-    <t>Movie12</t>
-  </si>
-  <si>
     <t>Password@12345</t>
+  </si>
+  <si>
+    <t>LoginType</t>
+  </si>
+  <si>
+    <t>Emailid</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>laxmi.khanal@quadlabs.com</t>
+  </si>
+  <si>
+    <t>//test.quadlabs.net/SSO_Login</t>
+  </si>
+  <si>
+    <t>test.quadlabs.net</t>
+  </si>
+  <si>
+    <t>SSOLogin</t>
+  </si>
+  <si>
+    <t>ankur.yadav@quadlabs.com</t>
+  </si>
+  <si>
+    <t>ankur</t>
+  </si>
+  <si>
+    <t>ccode</t>
+  </si>
+  <si>
+    <t>Test Project Name travog</t>
+  </si>
+  <si>
+    <t>SelectAllType</t>
+  </si>
+  <si>
+    <t>CostCenter</t>
+  </si>
+  <si>
+    <t>Traveler</t>
+  </si>
+  <si>
+    <t>Ankur Yadav</t>
+  </si>
+  <si>
+    <t>MarkStatus</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>UBER</t>
+  </si>
+  <si>
+    <t>Uber</t>
+  </si>
+  <si>
+    <t>Miles</t>
+  </si>
+  <si>
+    <t>SSO Login</t>
+  </si>
+  <si>
+    <t>Manali Trip</t>
+  </si>
+  <si>
+    <t>Hotel</t>
   </si>
 </sst>
 </file>
@@ -574,33 +633,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93D712F-96AB-4A28-A9EF-F2C73D8BB77C}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -611,147 +673,244 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1">
         <v>2000</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="N3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P2" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>28</v>
+      <c r="P3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{0A240D4F-A91F-48F4-B2DB-634436FC652C}">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R3" xr:uid="{0A240D4F-A91F-48F4-B2DB-634436FC652C}">
       <formula1>"SelectAllType,SearchType"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{C42D8072-032C-4E81-8B51-7DEE26D19540}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q3" xr:uid="{C42D8072-032C-4E81-8B51-7DEE26D19540}">
       <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler,Project,CostCenter,Division"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{6B63188C-85E0-42CD-9E54-9919631DB4F1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{6B63188C-85E0-42CD-9E54-9919631DB4F1}">
       <formula1>"SelectAll,ClearAll,CategorySelect"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{2BA26AB9-1D99-4E2C-97ED-E995C5706A40}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{2BA26AB9-1D99-4E2C-97ED-E995C5706A40}">
       <formula1>"AUD (Australian Dollars),BHD (Dinars (Bahrain)),IQD (Dinars (Iraq)),USD (Dollars (U.S.)),VND (Dongs (Vietnam)),INR (Indian Rupees),IDR (Indonesian Rupiahs),BRL (Reals (Brasil)),OMR (Rial Omanis),SAR (Riyals (Saudi Arabia)),ZAR (South African Rands)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{CF8F1C95-0485-4F47-A2E5-F83C1FE90981}">
+      <formula1>"Old Url,SSO Login"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{816DA501-BF0A-453A-8A49-29ABC0D8B1F9}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{24DCD205-25E5-4421-9F58-38B41BF0A95A}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{24DCD205-25E5-4421-9F58-38B41BF0A95A}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{40BD9985-29BE-4206-8BCB-EA4EEC99657D}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{36B68D14-4D4A-4D16-816A-D4561E238A8D}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{0D19ADA8-1C3E-4FCC-B85C-042525F02FFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170CB9B1-4C31-4EF7-9076-959CAD8DA0EB}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A99967-EDD0-4742-A392-5B021BBDEF73}">
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -762,116 +921,239 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>35</v>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3000</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1">
-        <v>2</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>28</v>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1">
+        <v>4000</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{D3DB4D7B-FEBB-40A5-9C7C-DAA1B7742B46}">
-      <formula1>"KM,Miles"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{FAF79F32-EC07-44BB-8839-8EE27EF2FBE2}">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{EB15B452-845B-41E4-9CCD-6E8604AE51D1}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3" xr:uid="{211ED6CD-82A7-4A87-8F45-8B378D44484B}">
+      <formula1>"AUD (Australian Dollars),BHD (Dinars (Bahrain)),IQD (Dinars (Iraq)),USD (Dollars (U.S.)),VND (Dongs (Vietnam)),INR (Indian Rupees),IDR (Indonesian Rupiahs),BRL (Reals (Brasil)),OMR (Rial Omanis),SAR (Riyals (Saudi Arabia)),ZAR (South African Rands)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{2088D07F-9B50-4E19-91F1-9FD38F888922}">
+      <formula1>"SelectAll,ClearAll,CategorySelect"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q3" xr:uid="{33BFEA81-149D-486C-B073-4CB401E7B5FB}">
       <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler,Project,CostCenter,Division"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{3909273F-94D4-45BA-8821-5277109904AB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R3" xr:uid="{A5B9BE0C-89DD-4044-8C10-E723D0F20801}">
       <formula1>"SelectAllType,SearchType"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{BF2304FF-DF20-43EE-9BFC-FC95E7A7DF90}">
+      <formula1>"Old Url,SSOLogin"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{3DAFAE3D-9F99-4560-A632-066EA00BFE12}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{EA129476-863D-4F6C-B97B-1FF77A844A2A}"/>
+    <hyperlink ref="E2" r:id="rId2" display="laxmi.khanal@quadlabs.com" xr:uid="{A8F0705A-C71B-4E11-9401-ADEC9328667A}"/>
+    <hyperlink ref="H3" r:id="rId3" xr:uid="{05354D38-19F8-4791-B44E-973B311C9806}"/>
+    <hyperlink ref="E3" r:id="rId4" display="laxmi.khanal@quadlabs.com" xr:uid="{C42C6F32-05F5-4C49-8EB2-3AC092BDE057}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9211EBE1-D17B-45BD-8FA9-3876669399FE}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170CB9B1-4C31-4EF7-9076-959CAD8DA0EB}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D1" sqref="D1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -882,120 +1164,145 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>41</v>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="1">
-        <v>2</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="K2" s="1">
-        <v>10</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2500</v>
+        <v>1000</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{7DBFD603-2B9B-4B95-B625-AEF30F116C54}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{D3DB4D7B-FEBB-40A5-9C7C-DAA1B7742B46}">
+      <formula1>"KM,Miles"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{FAF79F32-EC07-44BB-8839-8EE27EF2FBE2}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler,Project,CostCenter,Division"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{3909273F-94D4-45BA-8821-5277109904AB}">
       <formula1>"SelectAllType,SearchType"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{CB3AC5F1-927C-4E3F-8FCB-E9A4BDFECA45}">
-      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler,Project,CostCenter,Division"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{F9BC68AA-2437-4508-934F-FBFB26C30030}">
-      <formula1>"Travel,Non-Travel"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{8F193F94-41D2-4276-9456-772CD2DC63EC}">
+      <formula1>"Old Url,SSOLogin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{469C8447-086B-4450-8E14-7EDCAB434566}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{6FA63B06-C484-4016-B06D-F5BF8F413B02}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{3DAFAE3D-9F99-4560-A632-066EA00BFE12}"/>
+    <hyperlink ref="E2" r:id="rId2" display="laxmi.khanal@quadlabs.com" xr:uid="{E52EEEEF-025D-4633-9A24-69A5A2FE1487}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F525FAD2-6499-41EA-BAEC-EC34B2CE3542}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9211EBE1-D17B-45BD-8FA9-3876669399FE}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1006,81 +1313,410 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>52</v>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1">
-        <v>500000</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="1">
-        <v>2</v>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>54</v>
+        <v>22</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="1">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2500</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{8873F811-76E2-445F-A11B-F526FACF2247}">
-      <formula1>"Monthly,Quarterly,Yearly,Trip Basis"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{8D64986F-8455-49D4-820E-01D0486B4960}">
-      <formula1>"Department,Project,CostCenter"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{E41E6A05-63BA-4713-A8A4-11C46F810E78}">
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{7DBFD603-2B9B-4B95-B625-AEF30F116C54}">
       <formula1>"SelectAllType,SearchType"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{CB3AC5F1-927C-4E3F-8FCB-E9A4BDFECA45}">
+      <formula1>"Corporate,Corporate-Branch,Department,Designation,Grade,Traveler,Project,CostCenter,Division"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{F9BC68AA-2437-4508-934F-FBFB26C30030}">
+      <formula1>"Travel,Non-Travel"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{14DA045B-257E-4801-855D-FFAD73E59E76}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{D077B842-806D-472C-9BFD-D8FB42AFE834}">
+      <formula1>"Old Url,SSOLogin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{40E55FEB-3E95-4557-B2EB-161AC49D4295}">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{7631EF6E-900B-4EBB-B042-53B020AA70C8}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{6FA63B06-C484-4016-B06D-F5BF8F413B02}"/>
+    <hyperlink ref="E2" r:id="rId2" display="laxmi.khanal@quadlabs.com" xr:uid="{B3678BCD-5491-4084-961E-F1CB6FFF80BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F525FAD2-6499-41EA-BAEC-EC34B2CE3542}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="1">
+        <v>520000</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{8873F811-76E2-445F-A11B-F526FACF2247}">
+      <formula1>"Monthly,Quarterly,Yearly,Trip Basis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{8D64986F-8455-49D4-820E-01D0486B4960}">
+      <formula1>"Department,Project,CostCenter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{E41E6A05-63BA-4713-A8A4-11C46F810E78}">
+      <formula1>"SelectAllType,SearchType"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{E9864E2A-91EB-4416-9694-43EBFDFE6236}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{7B9B07EC-DD37-4AAA-9F8E-4902065F2DBB}">
+      <formula1>"Old Url,SSOLogin"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{7631EF6E-900B-4EBB-B042-53B020AA70C8}"/>
+    <hyperlink ref="E2" r:id="rId2" display="laxmi.khanal@quadlabs.com" xr:uid="{D1B2040E-4709-4038-BECB-74826975AE74}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31A15E8-897C-4EBB-8CE1-F21A81292CED}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="1">
+        <v>550000</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{86169337-2029-4740-98A9-367288B0C774}">
+      <formula1>"Old Url,SSOLogin"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{AB9362DC-1CBA-4E7C-8B07-7E07117E7E61}">
+      <formula1>"laxmi.khanal@quadlabs.com,ankur.yadav@quadlabs.com"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{1DF14740-891C-4F7D-9E28-6F7B1B9B41A6}">
+      <formula1>"SelectAllType,SearchType"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2" xr:uid="{43D446F1-5FC2-4820-B828-262EFB7DB213}">
+      <formula1>"Department,Project,CostCenter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{025BE812-17C3-4022-91C1-1019E238D2DE}">
+      <formula1>"Monthly,Quarterly,Yearly,Trip Basis"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{8641AAFA-6499-4FCB-B781-7B2C92CB1D95}">
+      <formula1>"//test.quadlabs.net/SSO_Login,//test.quadlabs.net/sbt/"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{55BBB7DC-F55D-49C3-9E75-429E71C9EC9C}"/>
+    <hyperlink ref="E2" r:id="rId2" display="laxmi.khanal@quadlabs.com" xr:uid="{EF1A66F3-342C-443E-A88A-F2CEE0641574}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>